<commit_message>
added create share skills
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaik\Downloads\marsframework-master\marsframework-master\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD1F249-7E88-477B-AF17-C0E5D25DC52A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24C4963-6F53-4FC4-94D0-ACDC220B4633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37530" yWindow="2325" windowWidth="18240" windowHeight="16785" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
     <sheet name="SignIn" sheetId="1" r:id="rId2"/>
     <sheet name="Profile" sheetId="2" r:id="rId3"/>
+    <sheet name="EnterShareSkill" sheetId="4" r:id="rId4"/>
+    <sheet name="EditShareSkill" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Url</t>
   </si>
@@ -120,10 +122,61 @@
     <t>3 years as Oracle Developer and 2 years as Project Management Operations Lead</t>
   </si>
   <si>
-    <t xml:space="preserve">mvpstudio.qa@gmail.com </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SydneyQa2018 </t>
+    <t>mvpstudio.qa@gmail.com</t>
+  </si>
+  <si>
+    <t>SydneyQa2018</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>StartTime</t>
+  </si>
+  <si>
+    <t>EndTime</t>
+  </si>
+  <si>
+    <t>SkillExchange</t>
+  </si>
+  <si>
+    <t>CreditAmount</t>
+  </si>
+  <si>
+    <t>Aisha</t>
+  </si>
+  <si>
+    <t>Learning Coding</t>
+  </si>
+  <si>
+    <t>#Coding</t>
+  </si>
+  <si>
+    <t>#java</t>
+  </si>
+  <si>
+    <t>Event Title</t>
+  </si>
+  <si>
+    <t>Scrum Meeting</t>
+  </si>
+  <si>
+    <t>EventDescription</t>
+  </si>
+  <si>
+    <t>Meeting to be attended</t>
   </si>
 </sst>
 </file>
@@ -176,10 +229,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -580,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -711,4 +765,103 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62BC598-6354-4FB3-96B2-F83D377EF408}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="3">
+        <v>43794</v>
+      </c>
+      <c r="I2" s="3">
+        <v>43794</v>
+      </c>
+      <c r="M2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8CD366-4483-428E-B8BE-1947BB78560B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Addes Start Date And End Date Of Available Days
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaik\Downloads\marsframework-master\marsframework-master\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2619CEA-C582-4A14-A6F5-DB76CC76695B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1354E76B-3D74-4E02-92DE-A8F3EA5A27B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43305" yWindow="1080" windowWidth="18240" windowHeight="16785" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32055" yWindow="945" windowWidth="18240" windowHeight="16785" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <t>Url</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>Code</t>
+  </si>
+  <si>
+    <t>10/12/2019</t>
+  </si>
+  <si>
+    <t>15/12/2019</t>
   </si>
 </sst>
 </file>
@@ -242,7 +248,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -780,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62BC598-6354-4FB3-96B2-F83D377EF408}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F10:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -840,11 +846,11 @@
       <c r="F2" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="3">
-        <v>43794</v>
-      </c>
-      <c r="I2" s="3">
-        <v>43794</v>
+      <c r="H2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="M2" t="s">
         <v>49</v>
@@ -858,6 +864,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -865,7 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8CD366-4483-428E-B8BE-1947BB78560B}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>